<commit_message>
changed penalty method to use steepest descent method
</commit_message>
<xml_diff>
--- a/03-lab/output/penalty_method_0_0.xlsx
+++ b/03-lab/output/penalty_method_0_0.xlsx
@@ -89,7 +89,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.25</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -109,7 +109,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.125</v>
+        <v>0.044999999999999998</v>
       </c>
       <c r="B3" s="0">
         <v>0</v>
@@ -129,7 +129,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.0625</v>
+        <v>0.0135</v>
       </c>
       <c r="B4" s="0">
         <v>0</v>
@@ -149,7 +149,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.03125</v>
+        <v>0.0040499999999999998</v>
       </c>
       <c r="B5" s="0">
         <v>0</v>

</xml_diff>